<commit_message>
update dynamicModel.js for assign correct datatype[int , float , varchar , date]
</commit_message>
<xml_diff>
--- a/backend/uploads/Purchases_Complex.xlsx
+++ b/backend/uploads/Purchases_Complex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\R.Sanjay\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC7BEBA-F728-4992-901F-170E793B28CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AEF162-E03D-4D5A-A694-633FFBEDCFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,18 +454,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="33.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -482,7 +483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5</v>
       </c>
@@ -500,7 +501,7 @@
         <v>45945</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6</v>
       </c>
@@ -518,7 +519,7 @@
         <v>45945</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7</v>
       </c>
@@ -536,7 +537,7 @@
         <v>45945</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8</v>
       </c>
@@ -554,7 +555,7 @@
         <v>45945</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10</v>
       </c>
@@ -572,7 +573,7 @@
         <v>45945</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>11</v>
       </c>
@@ -590,7 +591,7 @@
         <v>45945</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>12</v>
       </c>
@@ -608,7 +609,7 @@
         <v>45945</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>13</v>
       </c>
@@ -625,7 +626,7 @@
         <v>45955</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>14</v>
       </c>
@@ -642,7 +643,7 @@
         <v>45956</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>15</v>
       </c>
@@ -659,7 +660,7 @@
         <v>45957</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>16</v>
       </c>
@@ -676,7 +677,7 @@
         <v>45958</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>17</v>
       </c>
@@ -693,7 +694,7 @@
         <v>45959</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>18</v>
       </c>
@@ -709,8 +710,9 @@
       <c r="E14" s="2">
         <v>45960</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>19</v>
       </c>
@@ -727,7 +729,7 @@
         <v>45961</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>20</v>
       </c>

</xml_diff>